<commit_message>
Refactor code for improved readability and maintainability; remove unnecessary whitespace and debug comments
</commit_message>
<xml_diff>
--- a/public/import/template_nilai.xlsx
+++ b/public/import/template_nilai.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\laravel\generasijuara-web\public\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\generasijuara-web\public\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1C38AE-1D71-42B3-83A9-5ABBAF8955C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269A907E-0682-4A53-9F69-AEB7456DFFB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,14 +35,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -575,125 +575,125 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -981,142 +981,142 @@
       <selection activeCell="I11" sqref="I11:J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.9296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.06640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.53125" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.73046875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.19921875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.265625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.9296875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.796875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="9.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.06640625" style="1"/>
-    <col min="25" max="25" width="9.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.26953125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.90625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.81640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.08984375" style="1"/>
+    <col min="25" max="25" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="22" style="1" customWidth="1"/>
-    <col min="27" max="27" width="19.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.06640625" style="1"/>
+    <col min="27" max="27" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41" t="s">
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41" t="s">
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="72"/>
+      <c r="T1" s="72"/>
+      <c r="U1" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
-      <c r="X1" s="41"/>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="41"/>
-      <c r="AA1" s="42" t="s">
+      <c r="V1" s="72"/>
+      <c r="W1" s="72"/>
+      <c r="X1" s="72"/>
+      <c r="Y1" s="72"/>
+      <c r="Z1" s="72"/>
+      <c r="AA1" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="AB1" s="42"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="44" t="s">
+      <c r="AB1" s="73"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A2" s="70"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44" t="s">
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="43" t="s">
+      <c r="N2" s="75"/>
+      <c r="O2" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43" t="s">
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="43"/>
-      <c r="U2" s="45" t="s">
+      <c r="T2" s="74"/>
+      <c r="U2" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45" t="s">
+      <c r="V2" s="76"/>
+      <c r="W2" s="76"/>
+      <c r="X2" s="76"/>
+      <c r="Y2" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="Z2" s="45"/>
-      <c r="AA2" s="42"/>
-      <c r="AB2" s="42"/>
-    </row>
-    <row r="3" spans="1:28" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="40"/>
+      <c r="Z2" s="76"/>
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
+    </row>
+    <row r="3" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="70"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="71"/>
       <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" s="26"/>
       <c r="B4" s="26"/>
       <c r="C4" s="7"/>
@@ -1208,20 +1208,20 @@
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A5" s="46">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A5" s="66">
         <v>1</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="68">
         <v>201903001</v>
       </c>
-      <c r="D5" s="49">
+      <c r="D5" s="69">
         <v>2119995424</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="68" t="s">
         <v>40</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -1303,12 +1303,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A6" s="46"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="48"/>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A6" s="66"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="68"/>
       <c r="F6" s="8" t="s">
         <v>24</v>
       </c>
@@ -1388,12 +1388,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A7" s="46"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="48"/>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A7" s="66"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="68"/>
       <c r="F7" s="8" t="s">
         <v>26</v>
       </c>
@@ -1469,12 +1469,12 @@
       <c r="AA7" s="36"/>
       <c r="AB7" s="36"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A8" s="46"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="48"/>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A8" s="66"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="68"/>
       <c r="F8" s="8" t="s">
         <v>28</v>
       </c>
@@ -1550,12 +1550,12 @@
       <c r="AA8" s="36"/>
       <c r="AB8" s="36"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A9" s="46"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="48"/>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A9" s="66"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="68"/>
       <c r="F9" s="8" t="s">
         <v>30</v>
       </c>
@@ -1631,12 +1631,12 @@
       <c r="AA9" s="36"/>
       <c r="AB9" s="36"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A10" s="46"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="48"/>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A10" s="66"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="68"/>
       <c r="F10" s="8" t="s">
         <v>31</v>
       </c>
@@ -1712,23 +1712,23 @@
       <c r="AA10" s="36"/>
       <c r="AB10" s="36"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A11" s="46"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="75" t="s">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A11" s="66"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="75"/>
-      <c r="K11" s="76" t="s">
+      <c r="J11" s="48"/>
+      <c r="K11" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="76"/>
+      <c r="L11" s="49"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
@@ -1746,15 +1746,15 @@
       <c r="AA11" s="16"/>
       <c r="AB11" s="16"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A12" s="46"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A12" s="66"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
       <c r="I12" s="17" t="s">
         <v>20</v>
       </c>
@@ -1784,12 +1784,12 @@
       <c r="AA12" s="16"/>
       <c r="AB12" s="16"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A13" s="46"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="48"/>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A13" s="66"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="68"/>
       <c r="F13" s="8" t="s">
         <v>33</v>
       </c>
@@ -1830,12 +1830,12 @@
       <c r="AA13" s="16"/>
       <c r="AB13" s="16"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A14" s="46"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="48"/>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A14" s="66"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="68"/>
       <c r="F14" s="8" t="s">
         <v>34</v>
       </c>
@@ -1876,12 +1876,12 @@
       <c r="AA14" s="16"/>
       <c r="AB14" s="16"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A15" s="46"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="48"/>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A15" s="66"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="68"/>
       <c r="F15" s="8" t="s">
         <v>35</v>
       </c>
@@ -1922,12 +1922,12 @@
       <c r="AA15" s="16"/>
       <c r="AB15" s="16"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A16" s="46"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="48"/>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A16" s="66"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="68"/>
       <c r="F16" s="8" t="s">
         <v>38</v>
       </c>
@@ -1968,12 +1968,12 @@
       <c r="AA16" s="16"/>
       <c r="AB16" s="16"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A17" s="46"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="48"/>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A17" s="66"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="68"/>
       <c r="F17" s="8" t="s">
         <v>36</v>
       </c>
@@ -2014,12 +2014,12 @@
       <c r="AA17" s="16"/>
       <c r="AB17" s="16"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A18" s="46"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="48"/>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A18" s="66"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="68"/>
       <c r="F18" s="8" t="s">
         <v>37</v>
       </c>
@@ -2060,7 +2060,7 @@
       <c r="AA18" s="16"/>
       <c r="AB18" s="16"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A19" s="28"/>
       <c r="B19" s="29"/>
       <c r="C19" s="28"/>
@@ -2090,20 +2090,20 @@
       <c r="AA19" s="25"/>
       <c r="AB19" s="25"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A20" s="50">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A20" s="51">
         <v>2</v>
       </c>
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="56">
+      <c r="C20" s="57">
         <v>202004107</v>
       </c>
-      <c r="D20" s="59" t="s">
+      <c r="D20" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="62" t="s">
+      <c r="E20" s="63" t="s">
         <v>41</v>
       </c>
       <c r="F20" s="8" t="s">
@@ -2185,12 +2185,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A21" s="51"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="63"/>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A21" s="52"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="64"/>
       <c r="F21" s="8" t="s">
         <v>24</v>
       </c>
@@ -2270,12 +2270,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A22" s="51"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="63"/>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A22" s="52"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="64"/>
       <c r="F22" s="8" t="s">
         <v>26</v>
       </c>
@@ -2351,12 +2351,12 @@
       <c r="AA22" s="36"/>
       <c r="AB22" s="36"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A23" s="51"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="63"/>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A23" s="52"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="64"/>
       <c r="F23" s="8" t="s">
         <v>28</v>
       </c>
@@ -2432,12 +2432,12 @@
       <c r="AA23" s="36"/>
       <c r="AB23" s="36"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A24" s="51"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="63"/>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A24" s="52"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="64"/>
       <c r="F24" s="8" t="s">
         <v>30</v>
       </c>
@@ -2513,12 +2513,12 @@
       <c r="AA24" s="36"/>
       <c r="AB24" s="36"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A25" s="51"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="63"/>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A25" s="52"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="64"/>
       <c r="F25" s="8" t="s">
         <v>31</v>
       </c>
@@ -2594,23 +2594,23 @@
       <c r="AA25" s="36"/>
       <c r="AB25" s="36"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A26" s="51"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="71" t="s">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A26" s="52"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="72"/>
-      <c r="K26" s="73" t="s">
+      <c r="J26" s="45"/>
+      <c r="K26" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="L26" s="74"/>
+      <c r="L26" s="47"/>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
       <c r="O26" s="16"/>
@@ -2628,15 +2628,15 @@
       <c r="AA26" s="16"/>
       <c r="AB26" s="16"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A27" s="51"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="70"/>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A27" s="52"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="43"/>
       <c r="I27" s="17" t="s">
         <v>20</v>
       </c>
@@ -2666,12 +2666,12 @@
       <c r="AA27" s="16"/>
       <c r="AB27" s="16"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A28" s="51"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="63"/>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A28" s="52"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="64"/>
       <c r="F28" s="8" t="s">
         <v>33</v>
       </c>
@@ -2712,12 +2712,12 @@
       <c r="AA28" s="16"/>
       <c r="AB28" s="16"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A29" s="51"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="63"/>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A29" s="52"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="64"/>
       <c r="F29" s="8" t="s">
         <v>34</v>
       </c>
@@ -2758,12 +2758,12 @@
       <c r="AA29" s="16"/>
       <c r="AB29" s="16"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A30" s="51"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="63"/>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A30" s="52"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="64"/>
       <c r="F30" s="8" t="s">
         <v>35</v>
       </c>
@@ -2804,12 +2804,12 @@
       <c r="AA30" s="16"/>
       <c r="AB30" s="16"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A31" s="51"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="63"/>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A31" s="52"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="64"/>
       <c r="F31" s="8" t="s">
         <v>38</v>
       </c>
@@ -2850,12 +2850,12 @@
       <c r="AA31" s="16"/>
       <c r="AB31" s="16"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A32" s="51"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="63"/>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A32" s="52"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="64"/>
       <c r="F32" s="8" t="s">
         <v>36</v>
       </c>
@@ -2896,12 +2896,12 @@
       <c r="AA32" s="16"/>
       <c r="AB32" s="16"/>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A33" s="52"/>
-      <c r="B33" s="55"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="64"/>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A33" s="53"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="65"/>
       <c r="F33" s="8" t="s">
         <v>37</v>
       </c>
@@ -2944,22 +2944,12 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="F26:H27"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F11:H12"/>
-    <mergeCell ref="A20:A33"/>
-    <mergeCell ref="B20:B33"/>
-    <mergeCell ref="C20:C33"/>
-    <mergeCell ref="D20:D33"/>
-    <mergeCell ref="E20:E33"/>
-    <mergeCell ref="A5:A18"/>
-    <mergeCell ref="B5:B18"/>
-    <mergeCell ref="C5:C18"/>
-    <mergeCell ref="D5:D18"/>
-    <mergeCell ref="E5:E18"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:N1"/>
@@ -2972,12 +2962,22 @@
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="O1:T1"/>
     <mergeCell ref="O2:R2"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="A5:A18"/>
+    <mergeCell ref="B5:B18"/>
+    <mergeCell ref="C5:C18"/>
+    <mergeCell ref="D5:D18"/>
+    <mergeCell ref="E5:E18"/>
+    <mergeCell ref="A20:A33"/>
+    <mergeCell ref="B20:B33"/>
+    <mergeCell ref="C20:C33"/>
+    <mergeCell ref="D20:D33"/>
+    <mergeCell ref="E20:E33"/>
+    <mergeCell ref="F26:H27"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F11:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>